<commit_message>
I edited the schedule and added myself to junit tests, use case diagrams, and sequence diagrams.
</commit_message>
<xml_diff>
--- a/cit360_document_schedule.xlsx
+++ b/cit360_document_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\cit_360_group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seth/Documents/NetBeans/cit_360_group/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A5D931-72C0-49E3-847A-08A444FAC06E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAB0897-E4EE-EE46-9DEE-AB8D15B56124}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37560" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment Schedule" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Assignment Schedule'!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="43">
   <si>
     <t>MON</t>
   </si>
@@ -158,6 +158,9 @@
   <si>
     <t>Ben Langston</t>
   </si>
+  <si>
+    <t>Seth Huntley</t>
+  </si>
 </sst>
 </file>
 
@@ -243,6 +246,7 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2618,11 +2622,11 @@
   </sheetPr>
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="8" width="17.5" customWidth="1"/>
@@ -2630,7 +2634,7 @@
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2641,15 +2645,15 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -2739,7 +2743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -2760,7 +2764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>7</v>
@@ -2781,15 +2785,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2812,7 +2816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2835,7 +2839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>7</v>
@@ -2879,7 +2883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
         <v>7</v>
@@ -2900,7 +2904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>7</v>
@@ -2921,15 +2925,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
         <v>6</v>
       </c>
@@ -2952,7 +2956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
@@ -2975,7 +2979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="6" t="s">
         <v>26</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
         <v>7</v>
@@ -3019,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>7</v>
@@ -3040,7 +3044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>7</v>
@@ -3061,15 +3065,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="5" t="s">
         <v>6</v>
       </c>
@@ -3092,7 +3096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="6" t="s">
         <v>27</v>
       </c>
@@ -3115,7 +3119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
         <v>28</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
         <v>7</v>
@@ -3159,7 +3163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
         <v>7</v>
@@ -3180,7 +3184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
         <v>7</v>
@@ -3201,15 +3205,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
@@ -3232,7 +3236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="6" t="s">
         <v>29</v>
       </c>
@@ -3243,7 +3247,7 @@
         <v>7</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>7</v>
@@ -3255,7 +3259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="6" t="s">
         <v>30</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
         <v>7</v>
@@ -3299,7 +3303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
         <v>7</v>
@@ -3320,7 +3324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>7</v>
@@ -3341,15 +3345,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="5" t="s">
         <v>6</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="6" t="s">
         <v>31</v>
       </c>
@@ -3383,7 +3387,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>7</v>
@@ -3395,7 +3399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="6" t="s">
         <v>32</v>
       </c>
@@ -3418,7 +3422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
         <v>7</v>
@@ -3439,7 +3443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
         <v>7</v>
@@ -3460,7 +3464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
         <v>7</v>
@@ -3481,15 +3485,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B56" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="5" t="s">
         <v>6</v>
       </c>
@@ -3512,7 +3516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="6" t="s">
         <v>33</v>
       </c>
@@ -3535,7 +3539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="6" t="s">
         <v>34</v>
       </c>
@@ -3546,7 +3550,7 @@
         <v>7</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>7</v>
@@ -3558,7 +3562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
         <v>7</v>
@@ -3579,7 +3583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
         <v>7</v>
@@ -3600,7 +3604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
         <v>7</v>
@@ -3621,15 +3625,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B65" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B67" s="5" t="s">
         <v>6</v>
       </c>
@@ -3652,7 +3656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B68" s="6" t="s">
         <v>35</v>
       </c>
@@ -3675,7 +3679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
         <v>7</v>
@@ -3696,7 +3700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
         <v>7</v>
@@ -3717,7 +3721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
         <v>7</v>
@@ -3738,7 +3742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
         <v>7</v>
@@ -3759,15 +3763,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B74" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B75" s="4"/>
     </row>
-    <row r="76" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B76" s="5" t="s">
         <v>6</v>
       </c>
@@ -3790,7 +3794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B77" s="6" t="s">
         <v>35</v>
       </c>
@@ -3813,7 +3817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
         <v>7</v>
@@ -3834,7 +3838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
         <v>7</v>
@@ -3855,7 +3859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
         <v>7</v>
@@ -3876,7 +3880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
         <v>7</v>
@@ -3897,15 +3901,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B83" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B85" s="5" t="s">
         <v>6</v>
       </c>
@@ -3928,7 +3932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B86" s="6" t="s">
         <v>35</v>
       </c>
@@ -3951,7 +3955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B87" s="6"/>
       <c r="C87" s="6" t="s">
         <v>7</v>
@@ -3972,7 +3976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
         <v>7</v>
@@ -3993,7 +3997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
         <v>7</v>
@@ -4014,7 +4018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
         <v>7</v>
@@ -4035,15 +4039,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B92" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B93" s="4"/>
     </row>
-    <row r="94" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B94" s="5" t="s">
         <v>6</v>
       </c>
@@ -4066,7 +4070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B95" s="6" t="s">
         <v>35</v>
       </c>
@@ -4089,7 +4093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="s">
         <v>7</v>
@@ -4110,7 +4114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B97" s="6"/>
       <c r="C97" s="6" t="s">
         <v>7</v>
@@ -4131,7 +4135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="s">
         <v>7</v>
@@ -4152,7 +4156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B99" s="6"/>
       <c r="C99" s="6" t="s">
         <v>7</v>
@@ -4173,15 +4177,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B101" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B102" s="4"/>
     </row>
-    <row r="103" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B103" s="5" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B104" s="6" t="s">
         <v>35</v>
       </c>
@@ -4227,7 +4231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B105" s="6" t="s">
         <v>36</v>
       </c>
@@ -4250,7 +4254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B106" s="6"/>
       <c r="C106" s="6" t="s">
         <v>7</v>
@@ -4271,7 +4275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B107" s="6"/>
       <c r="C107" s="6" t="s">
         <v>7</v>
@@ -4292,7 +4296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B108" s="6"/>
       <c r="C108" s="6" t="s">
         <v>7</v>
@@ -4313,13 +4317,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B111" s="4"/>
     </row>
-    <row r="112" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -4328,7 +4332,7 @@
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
     </row>
-    <row r="113" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
@@ -4337,7 +4341,7 @@
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
     </row>
-    <row r="114" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
@@ -4346,7 +4350,7 @@
       <c r="G114" s="6"/>
       <c r="H114" s="6"/>
     </row>
-    <row r="115" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
@@ -4355,7 +4359,7 @@
       <c r="G115" s="6"/>
       <c r="H115" s="6"/>
     </row>
-    <row r="116" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -4364,7 +4368,7 @@
       <c r="G116" s="6"/>
       <c r="H116" s="6"/>
     </row>
-    <row r="117" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
@@ -4373,7 +4377,7 @@
       <c r="G117" s="6"/>
       <c r="H117" s="6"/>
     </row>
-    <row r="119" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B119" s="7"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
@@ -4382,7 +4386,7 @@
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
     </row>
-    <row r="120" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B120" s="9"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
@@ -4391,7 +4395,7 @@
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
     </row>
-    <row r="121" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
@@ -4400,7 +4404,7 @@
       <c r="G121" s="8"/>
       <c r="H121" s="8"/>
     </row>
-    <row r="122" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B122" s="11"/>
       <c r="C122" s="12"/>
       <c r="D122" s="12"/>
@@ -4409,7 +4413,7 @@
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
     </row>
-    <row r="123" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B123" s="11"/>
       <c r="C123" s="12"/>
       <c r="D123" s="12"/>
@@ -4418,7 +4422,7 @@
       <c r="G123" s="8"/>
       <c r="H123" s="8"/>
     </row>
-    <row r="124" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B124" s="11"/>
       <c r="C124" s="12"/>
       <c r="D124" s="12"/>
@@ -4427,7 +4431,7 @@
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
     </row>
-    <row r="125" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B125" s="11"/>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
@@ -4436,7 +4440,7 @@
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
     </row>
-    <row r="126" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B126" s="13"/>
       <c r="C126" s="14"/>
       <c r="D126" s="14"/>
@@ -4445,12 +4449,12 @@
       <c r="G126" s="8"/>
       <c r="H126" s="8"/>
     </row>
-    <row r="127" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F127" s="8"/>
       <c r="G127" s="8"/>
       <c r="H127" s="8"/>
     </row>
-    <row r="128" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F128" s="8"/>
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>

</xml_diff>